<commit_message>
save registration and delete profile script
</commit_message>
<xml_diff>
--- a/src/test/java/abpw/testData/abpwDataSet.xlsx
+++ b/src/test/java/abpw/testData/abpwDataSet.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8250" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="4710" windowWidth="12450"/>
   </bookViews>
   <sheets>
-    <sheet name="Generic" sheetId="2" r:id="rId1"/>
-    <sheet name="Registration" sheetId="3" r:id="rId2"/>
-    <sheet name="Profiles" sheetId="6" r:id="rId3"/>
-    <sheet name="PC" sheetId="4" r:id="rId4"/>
-    <sheet name="PP" sheetId="7" r:id="rId5"/>
+    <sheet name="Generic" r:id="rId1" sheetId="2"/>
+    <sheet name="Registration" r:id="rId2" sheetId="3"/>
+    <sheet name="Profiles" r:id="rId3" sheetId="6"/>
+    <sheet name="PC" r:id="rId4" sheetId="4"/>
+    <sheet name="PP" r:id="rId5" sheetId="7"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:B13"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="4">
   <si>
     <t>USER NAME</t>
   </si>
@@ -72,7 +72,7 @@
     <t>Email</t>
   </si>
   <si>
-    <t>test.testwebauto025@yopmail.com</t>
+    <t>test.testwebauto031@yopmail.com</t>
   </si>
   <si>
     <t>Religion</t>
@@ -111,7 +111,7 @@
     <t>Create User AWID</t>
   </si>
   <si>
-    <t>AW42521245</t>
+    <t>AW75356707</t>
   </si>
   <si>
     <t>PeopleUsuallyTellMe</t>
@@ -409,6 +409,18 @@
   </si>
   <si>
     <t>Kolkata-CITY</t>
+  </si>
+  <si>
+    <t>AW85949526</t>
+  </si>
+  <si>
+    <t>AW27724621</t>
+  </si>
+  <si>
+    <t>AW24608735</t>
+  </si>
+  <si>
+    <t>AW79934728</t>
   </si>
 </sst>
 </file>
@@ -416,8 +428,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -483,6 +495,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -497,10 +539,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -512,6 +555,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -520,26 +607,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -552,67 +624,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -647,19 +659,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -671,163 +833,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -989,32 +1001,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1025,15 +1011,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1052,283 +1029,318 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="176">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="177">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="178">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="179">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="13" fillId="9" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="12" fillId="0" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="15" fillId="16" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="23" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="12" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="17" fillId="0" fontId="24" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="24" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="14" fillId="13" fontId="20" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="34" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="22" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="18" fillId="30" fontId="25" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="14" fillId="30" fontId="27" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="11" fillId="0" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="16" fillId="0" fontId="21" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="26" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="13" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="41">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="10"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
+    <cellStyle builtinId="10" name="Note" xfId="9"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1342,10 +1354,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1509,21 +1521,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1540,7 +1552,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1593,19 +1605,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="39.1428571428571" style="30" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.2857142857143" style="30" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.14285714285714" style="30" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="30" width="39.1428571428571" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="30" width="36.2857142857143" collapsed="true"/>
+    <col min="3" max="16384" style="30" width="9.14285714285714" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1625,28 +1637,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.25" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="28" style="11" customWidth="1"/>
-    <col min="2" max="2" width="52.1428571428571" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="9.14285714285714" style="11"/>
+    <col min="1" max="1" customWidth="true" style="11" width="28.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="11" width="52.1428571428571" collapsed="true"/>
+    <col min="3" max="16384" style="11" width="9.14285714285714" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="31" customFormat="1" spans="1:2">
+    <row customFormat="1" r="1" s="31" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1752,25 +1764,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" display="test.testwebauto025@yopmail.com"/>
+    <hyperlink display="test.testwebauto031@yopmail.com" r:id="rId1" ref="B8" tooltip="mailto:test.testwebauto031@yopmail.com"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="B7 G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="1" outlineLevelRow="1"/>
   <cols>
-    <col min="2" max="2" width="36.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="36.5714285714286" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1786,19 +1798,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
@@ -1806,10 +1818,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.25" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="32.8571428571429" style="11" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.2857142857143" style="11" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.5714285714286" style="11" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.14285714285714" style="11" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="11" width="32.8571428571429" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="11" width="36.2857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="11" width="30.5714285714286" collapsed="true"/>
+    <col min="4" max="16384" style="11" width="9.14285714285714" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2247,29 +2259,29 @@
     <mergeCell ref="C27:C34"/>
     <mergeCell ref="C36:C46"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="16.5" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="16.5" outlineLevelCol="2" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="26.5714285714286" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.4285714285714" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.5714285714286" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.14285714285714" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="26.5714285714286" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="29.4285714285714" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="31.5714285714286" collapsed="true"/>
+    <col min="4" max="16384" style="1" width="9.14285714285714" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" spans="1:2">
+    <row ht="17.25" r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2337,7 +2349,7 @@
   <mergeCells count="1">
     <mergeCell ref="C2:C7"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>